<commit_message>
updated report docs (#7643)
</commit_message>
<xml_diff>
--- a/docs/data/advanced_data_example_v20171206.xlsx
+++ b/docs/data/advanced_data_example_v20171206.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{701F6DF9-0D5D-0D49-8A8F-7D1E70F75A63}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10820" yWindow="-19000" windowWidth="25360" windowHeight="14620" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="-25360" yWindow="-8060" windowWidth="25360" windowHeight="14620" tabRatio="679" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="root_hospital_cities" sheetId="1" r:id="rId1"/>
-    <sheet name="root_hospital_patients" sheetId="2" r:id="rId2"/>
-    <sheet name="root_hospital_users" sheetId="3" r:id="rId3"/>
+    <sheet name="cities" sheetId="1" r:id="rId1"/>
+    <sheet name="patients" sheetId="2" r:id="rId2"/>
+    <sheet name="users" sheetId="3" r:id="rId3"/>
     <sheet name="attributes" sheetId="4" r:id="rId4"/>
     <sheet name="entities" sheetId="5" r:id="rId5"/>
-    <sheet name="packages" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>cityName</t>
   </si>
@@ -152,9 +157,6 @@
     <t>whether user is active</t>
   </si>
   <si>
-    <t>package</t>
-  </si>
-  <si>
     <t>extends</t>
   </si>
   <si>
@@ -173,31 +175,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>my main package</t>
-  </si>
-  <si>
-    <t>sub package holding entities to describe all kinds of persons</t>
-  </si>
-  <si>
     <t>list of cities</t>
-  </si>
-  <si>
-    <t>root_hospital_cities</t>
-  </si>
-  <si>
-    <t>root_hospital_patients</t>
-  </si>
-  <si>
-    <t>root_hospital_users</t>
-  </si>
-  <si>
-    <t>root_hospital</t>
   </si>
   <si>
     <t>lat</t>
@@ -245,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -364,6 +342,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -688,29 +674,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3">
         <v>40.712783999999999</v>
@@ -719,7 +705,7 @@
         <v>-74.005941000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -741,16 +727,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -767,15 +753,15 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -784,18 +770,18 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -810,9 +796,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -821,10 +807,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -841,16 +827,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -867,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -875,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -884,12 +870,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -898,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -923,14 +909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
@@ -939,9 +925,9 @@
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -962,12 +948,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -979,35 +965,35 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1035,7 +1021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1046,12 +1032,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -1060,57 +1046,57 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1122,12 +1108,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -1147,23 +1133,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>42</v>
@@ -1172,114 +1157,48 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="b">
+      <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
+      <c r="D5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>